<commit_message>
fixed non unique keys between 0648 and 0684
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_0684.xlsx
+++ b/bioSample/bioSample_0684.xlsx
@@ -230,10 +230,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -279,7 +279,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
@@ -287,7 +287,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
@@ -308,7 +308,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>18</v>
       </c>
@@ -316,7 +316,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -337,7 +337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>18</v>
       </c>
@@ -345,7 +345,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
@@ -366,7 +366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>18</v>
       </c>
@@ -374,7 +374,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -395,7 +395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>18</v>
       </c>
@@ -403,7 +403,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>14</v>
@@ -424,7 +424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>18</v>
       </c>
@@ -432,7 +432,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>14</v>
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>18</v>
       </c>
@@ -461,7 +461,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>14</v>
@@ -482,7 +482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>18</v>
       </c>
@@ -490,7 +490,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
@@ -511,7 +511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>18</v>
       </c>
@@ -519,7 +519,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>14</v>
@@ -540,7 +540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>18</v>
       </c>
@@ -548,7 +548,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
@@ -569,7 +569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>25</v>
       </c>
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
@@ -598,7 +598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>25</v>
       </c>
@@ -606,7 +606,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
@@ -627,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>25</v>
       </c>
@@ -635,7 +635,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>25</v>
       </c>
@@ -664,7 +664,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>14</v>
@@ -685,7 +685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>25</v>
       </c>
@@ -693,7 +693,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>14</v>
@@ -714,7 +714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>25</v>
       </c>
@@ -722,7 +722,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
@@ -743,7 +743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>25</v>
       </c>
@@ -751,7 +751,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>14</v>
@@ -772,7 +772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>25</v>
       </c>
@@ -780,7 +780,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>14</v>
@@ -801,6 +801,7 @@
         <v>3</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
updating g418 idnetified strains
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_0684.xlsx
+++ b/bioSample/bioSample_0684.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="30">
   <si>
     <t xml:space="preserve">harvestDate</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">CNAG_00440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G418</t>
   </si>
 </sst>
 </file>
@@ -121,6 +124,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -205,7 +209,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -214,7 +218,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.07"/>
@@ -746,6 +750,9 @@
       <c r="I17" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="J17" s="0" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -775,6 +782,9 @@
       <c r="I18" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="J18" s="0" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -803,6 +813,9 @@
       </c>
       <c r="I19" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>